<commit_message>
This is my Framework with Modified Datadriven and Logout commit
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetbanking/testData/LoginData.xlsx
+++ b/src/test/java/com/inetbanking/testData/LoginData.xlsx
@@ -19,12 +19,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+  <si>
+    <t>mngr83460</t>
+  </si>
+  <si>
+    <t>qAbUzyj</t>
+  </si>
   <si>
     <t>username</t>
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>mngr164225</t>
+  </si>
+  <si>
+    <t>jahetAp</t>
   </si>
   <si>
     <t>mngr168479</t>
@@ -423,7 +435,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,50 +446,50 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>